<commit_message>
Amtoli Input File Prep
Amtoli Input File Prep
</commit_message>
<xml_diff>
--- a/AEMostofa/Meherpur WD Division/P1/Amtoil Khal/XL_FILE_CROSS_SECTION/Amtoil khal Cross Section .xlsx
+++ b/AEMostofa/Meherpur WD Division/P1/Amtoil Khal/XL_FILE_CROSS_SECTION/Amtoil khal Cross Section .xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr showInkAnnotation="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Design_All_DC_5\AEMostofa\Meherpur WD Division\P1\Amtoil Khal\XL_FILE_CROSS_SECTION\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C264FFE-7431-4091-BFFD-E1DCD26B3BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" activeTab="3"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover " sheetId="18" r:id="rId1"/>
@@ -18,7 +24,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Long Section (2)'!$A$1:$Z$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'out fall'!$A$1:$K$149</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -160,7 +166,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
@@ -553,7 +559,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -683,43 +689,40 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -728,48 +731,44 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -778,13 +777,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -799,7 +798,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -823,9 +822,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -844,21 +840,24 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Comma 5" xfId="8"/>
+    <cellStyle name="Comma 5" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 11" xfId="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="5"/>
-    <cellStyle name="Normal 2 2 2" xfId="9"/>
-    <cellStyle name="Normal 3" xfId="10"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
-    <cellStyle name="Normal 4 3" xfId="6"/>
-    <cellStyle name="Normal 6" xfId="11"/>
-    <cellStyle name="Normal 6 2" xfId="4"/>
-    <cellStyle name="Normal 7" xfId="12"/>
-    <cellStyle name="Normal 8" xfId="7"/>
+    <cellStyle name="Normal 11" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 4 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 6" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 6 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 7" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 8" xfId="7" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -874,7 +873,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1351,7 +1350,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ADBD-4D0E-8FCF-D83BF74E06FC}"/>
             </c:ext>
@@ -1468,7 +1467,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1629,7 +1628,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-90E4-412E-87AB-4AB5FB93A160}"/>
             </c:ext>
@@ -1737,7 +1736,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-90E4-412E-87AB-4AB5FB93A160}"/>
             </c:ext>
@@ -1990,7 +1989,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2151,7 +2150,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5824-4FC9-8875-8C731901CCDC}"/>
             </c:ext>
@@ -2253,7 +2252,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5824-4FC9-8875-8C731901CCDC}"/>
             </c:ext>
@@ -2506,7 +2505,7 @@
 </file>
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2679,7 +2678,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FDE8-4A35-8A28-5334EA2655E3}"/>
             </c:ext>
@@ -2775,7 +2774,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FDE8-4A35-8A28-5334EA2655E3}"/>
             </c:ext>
@@ -3028,7 +3027,7 @@
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3159,7 +3158,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5BD1-426A-B600-2A6D384C4D21}"/>
             </c:ext>
@@ -3249,7 +3248,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5BD1-426A-B600-2A6D384C4D21}"/>
             </c:ext>
@@ -3502,7 +3501,7 @@
 </file>
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3669,7 +3668,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CC40-441E-A0AD-0BA0C83BECBE}"/>
             </c:ext>
@@ -3765,7 +3764,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-CC40-441E-A0AD-0BA0C83BECBE}"/>
             </c:ext>
@@ -4018,7 +4017,7 @@
 </file>
 
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4185,7 +4184,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-827E-4EF8-AAD2-2D13BF203523}"/>
             </c:ext>
@@ -4311,7 +4310,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-827E-4EF8-AAD2-2D13BF203523}"/>
             </c:ext>
@@ -4564,7 +4563,7 @@
 </file>
 
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4689,7 +4688,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5A87-40B4-AE89-08296B8FE540}"/>
             </c:ext>
@@ -4779,7 +4778,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5A87-40B4-AE89-08296B8FE540}"/>
             </c:ext>
@@ -5032,7 +5031,7 @@
 </file>
 
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5201,7 +5200,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0A05-4450-84C8-9C327B3AC712}"/>
             </c:ext>
@@ -5334,7 +5333,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0A05-4450-84C8-9C327B3AC712}"/>
             </c:ext>
@@ -5475,7 +5474,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0A05-4450-84C8-9C327B3AC712}"/>
             </c:ext>
@@ -5609,7 +5608,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-0A05-4450-84C8-9C327B3AC712}"/>
             </c:ext>
@@ -5813,7 +5812,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6296,7 +6295,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FF7B-441E-A8EE-5FE5DC858E39}"/>
             </c:ext>
@@ -6413,7 +6412,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6616,7 +6615,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AB02-4AF9-BBE0-2FBFC159F966}"/>
             </c:ext>
@@ -6694,7 +6693,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-AB02-4AF9-BBE0-2FBFC159F966}"/>
             </c:ext>
@@ -6947,7 +6946,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7116,7 +7115,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F650-4CEA-AF4E-EAD36BD3BCC2}"/>
             </c:ext>
@@ -7194,7 +7193,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F650-4CEA-AF4E-EAD36BD3BCC2}"/>
             </c:ext>
@@ -7447,7 +7446,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7585,7 +7584,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-651F-4F3E-8AC3-58B74378DBDC}"/>
             </c:ext>
@@ -7670,7 +7669,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-651F-4F3E-8AC3-58B74378DBDC}"/>
             </c:ext>
@@ -7790,7 +7789,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-651F-4F3E-8AC3-58B74378DBDC}"/>
             </c:ext>
@@ -7880,7 +7879,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-651F-4F3E-8AC3-58B74378DBDC}"/>
             </c:ext>
@@ -8133,7 +8132,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8294,7 +8293,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-323F-4165-BD9D-F87A033AE2EF}"/>
             </c:ext>
@@ -8384,7 +8383,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-323F-4165-BD9D-F87A033AE2EF}"/>
             </c:ext>
@@ -8637,7 +8636,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8792,7 +8791,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E5D3-473A-BB26-BA2913E06798}"/>
             </c:ext>
@@ -8882,7 +8881,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-E5D3-473A-BB26-BA2913E06798}"/>
             </c:ext>
@@ -9135,7 +9134,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9314,7 +9313,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-37EE-47AA-9F37-07C565002E15}"/>
             </c:ext>
@@ -9440,7 +9439,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-37EE-47AA-9F37-07C565002E15}"/>
             </c:ext>
@@ -9693,7 +9692,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -9860,7 +9859,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7CE6-48E9-B9C7-F0E1FEBA1A5C}"/>
             </c:ext>
@@ -9956,7 +9955,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7CE6-48E9-B9C7-F0E1FEBA1A5C}"/>
             </c:ext>
@@ -10225,7 +10224,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -10293,7 +10298,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -10343,7 +10354,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ECD26149-C9AE-4D40-B10F-750C07B7E900}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECD26149-C9AE-4D40-B10F-750C07B7E900}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10353,7 +10364,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="74585" y="142082"/>
+          <a:off x="74714" y="142082"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10413,7 +10424,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{782A469D-7FEA-499A-B2CF-3AF76541F41E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{782A469D-7FEA-499A-B2CF-3AF76541F41E}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10423,7 +10434,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="75553" y="144662"/>
+          <a:off x="75682" y="144662"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10483,7 +10494,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{51B90191-9E2E-483C-B32B-0324FF181178}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B90191-9E2E-483C-B32B-0324FF181178}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10493,7 +10504,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="75650" y="149368"/>
+          <a:off x="75779" y="149368"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10553,7 +10564,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10563,7 +10574,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="74843" y="145725"/>
+          <a:off x="74972" y="145725"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10623,7 +10634,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10633,7 +10644,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="75644" y="163637"/>
+          <a:off x="75774" y="161208"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10693,7 +10704,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10703,7 +10714,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="75644" y="144794"/>
+          <a:off x="75774" y="142851"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10763,7 +10774,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10773,7 +10784,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="76129" y="135564"/>
+          <a:off x="76258" y="137022"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10833,7 +10844,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10843,7 +10854,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="75967" y="144794"/>
+          <a:off x="76096" y="142851"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10903,7 +10914,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10913,7 +10924,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="75967" y="144794"/>
+          <a:off x="76096" y="142851"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -10973,7 +10984,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{967A7FB0-D905-4A8C-89B5-EBEAC633915F}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -10983,7 +10994,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="75967" y="144794"/>
+          <a:off x="76096" y="142851"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -11047,7 +11058,7 @@
         <xdr:cNvPr id="30" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16C425A1-19E1-4C5A-B718-B5AAB4235228}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11085,7 +11096,7 @@
         <xdr:cNvPr id="31" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2600C943-0C5E-429D-95C5-FDE7D631707E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11123,7 +11134,7 @@
         <xdr:cNvPr id="34" name="Text Box 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BD39F621-B5F0-4DC5-A753-3F044490B542}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000022000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11353,7 +11364,7 @@
         <xdr:cNvPr id="35" name="TextBox 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B3543DEE-12A2-4D39-86DB-14A6543D5D2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000023000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11521,7 +11532,7 @@
         <xdr:cNvPr id="6" name="TextBox 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{49D8D0F4-14AC-4A6D-B858-A5D9EB48EDA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11731,7 +11742,7 @@
         <xdr:cNvPr id="7" name="TextBox 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA55B803-0DAA-482F-8C41-942A6547ED62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11943,7 +11954,7 @@
         <xdr:cNvPr id="8" name="TextBox 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89E25DD0-C8F6-4602-848E-F91786D3DFE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12133,7 +12144,7 @@
         <xdr:cNvPr id="2" name="Chart 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{88987468-3F82-4955-9231-3C81D4D858C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12171,7 +12182,7 @@
         <xdr:cNvPr id="3" name="Text Box 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6EE4D8EC-C077-4A85-AA15-B340E6DFF845}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12432,7 +12443,7 @@
         <xdr:cNvPr id="4" name="TextBox 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E74A58BD-FFCF-4FF7-B24C-47033912C084}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12605,7 +12616,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C1D9AC2-D8EF-4545-9AA5-1C4C27CA5EE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13124,7 +13135,7 @@
         <xdr:cNvPr id="2" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0D1823FC-888E-40DB-8EB3-678D4A1AC8F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13162,7 +13173,7 @@
         <xdr:cNvPr id="3" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7B37427C-A9E5-4566-A78D-278847FF9E62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13200,7 +13211,7 @@
         <xdr:cNvPr id="4" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{81BD830B-EC3A-4700-8E32-43CE03D1BD40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13238,7 +13249,7 @@
         <xdr:cNvPr id="5" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{71B0A7C4-C4BB-4B02-848B-4B7C6C6E1F3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13276,7 +13287,7 @@
         <xdr:cNvPr id="6" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{465D93ED-3C43-4554-9975-0F676D7D95C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13314,7 +13325,7 @@
         <xdr:cNvPr id="7" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E017171F-B85B-4DDD-A854-073430515FA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13352,7 +13363,7 @@
         <xdr:cNvPr id="8" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7614B940-4C60-4498-B6AA-A9DAAC447513}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13390,7 +13401,7 @@
         <xdr:cNvPr id="9" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ED49FAC9-3C53-43BB-93D2-3E9168F4214F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13423,7 +13434,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C4B5B904-831E-442B-BD8D-C05507FB8ABC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13624,7 +13635,7 @@
         <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B7825B1E-0E60-4A9A-AF66-1AC9B4C99061}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13865,7 +13876,7 @@
         <xdr:cNvPr id="12" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CE1FEBD4-9685-452E-8FE9-BA91BCA103DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13903,7 +13914,7 @@
         <xdr:cNvPr id="13" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{047CE50D-F67D-4A2D-B95C-8658235E82F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13941,7 +13952,7 @@
         <xdr:cNvPr id="14" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD1EE713-2CD5-4D06-B2F9-F83943FED263}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13979,7 +13990,7 @@
         <xdr:cNvPr id="15" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D31DC7C4-1DF7-4350-B1A5-C31C08A13362}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14017,7 +14028,7 @@
         <xdr:cNvPr id="16" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6E41AE3-AE0F-4317-9547-93222335E678}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14055,7 +14066,7 @@
         <xdr:cNvPr id="17" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9BECFB21-B2D5-45A8-A713-1778709A8D82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14088,7 +14099,7 @@
         <xdr:cNvPr id="28" name="TextBox 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{49D8D0F4-14AC-4A6D-B858-A5D9EB48EDA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14286,7 +14297,7 @@
         <xdr:cNvPr id="29" name="TextBox 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FA55B803-0DAA-482F-8C41-942A6547ED62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14510,7 +14521,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89E25DD0-C8F6-4602-848E-F91786D3DFE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14696,7 +14707,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2B92B1EC-EFBE-4903-8886-6AE33DA2A3E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B92B1EC-EFBE-4903-8886-6AE33DA2A3E6}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -14706,7 +14717,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="78476" y="152093"/>
+          <a:off x="75131" y="152239"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -14766,7 +14777,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E414D1BC-9DA7-4119-8D93-89281D7A4822}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E414D1BC-9DA7-4119-8D93-89281D7A4822}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -14776,7 +14787,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="74824" y="183391"/>
+          <a:off x="74953" y="183391"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -14836,7 +14847,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A4B4E647-D8DA-447E-AC0B-3A43469635B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4B4E647-D8DA-447E-AC0B-3A43469635B5}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -14846,7 +14857,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="76102" y="158476"/>
+          <a:off x="76257" y="158476"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -14901,7 +14912,7 @@
         <cdr:cNvPr id="2" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D2CBC91D-8C06-4DE0-965D-650E4DE24B07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2CBC91D-8C06-4DE0-965D-650E4DE24B07}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -14911,7 +14922,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="76102" y="158476"/>
+          <a:off x="76257" y="158476"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -14922,7 +14933,7 @@
           <cdr:cNvPr id="3" name="TextBox 14">
             <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BFC8796-0C33-433E-B22F-13A00497C312}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BFC8796-0C33-433E-B22F-13A00497C312}"/>
               </a:ext>
             </a:extLst>
           </cdr:cNvPr>
@@ -14977,7 +14988,7 @@
         <cdr:cNvPr id="6" name="Group 11">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D2CBC91D-8C06-4DE0-965D-650E4DE24B07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2CBC91D-8C06-4DE0-965D-650E4DE24B07}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -14987,7 +14998,7 @@
       </cdr:nvGrpSpPr>
       <cdr:grpSpPr bwMode="auto">
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
-          <a:off x="75811" y="146898"/>
+          <a:off x="75940" y="146898"/>
           <a:ext cx="0" cy="0"/>
           <a:chOff x="3400425" y="1304934"/>
           <a:chExt cx="1962165" cy="600066"/>
@@ -15320,15 +15331,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB48"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="S31" sqref="S31"/>
@@ -16170,7 +16181,7 @@
     <col min="16146" max="16384" width="8.88671875" style="66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="63"/>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -16184,1168 +16195,667 @@
       <c r="K1" s="64"/>
       <c r="L1" s="65"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="67"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="69"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L2" s="68"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="67"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="69"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L3" s="68"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="68"/>
-      <c r="Q4" s="68"/>
-    </row>
-    <row r="5" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102" t="s">
+      <c r="L4" s="68"/>
+    </row>
+    <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
-      <c r="E5" s="103"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="103"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="68"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="67"/>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L6" s="68"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="67"/>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="68"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L7" s="68"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="67"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L8" s="68"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="67"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="68"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="68"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L9" s="68"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="67"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="68"/>
-      <c r="K10" s="68"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="68"/>
-      <c r="O10" s="68"/>
-      <c r="P10" s="68" t="s">
+      <c r="L10" s="68"/>
+      <c r="P10" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="Q10" s="68"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="67"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="68"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L11" s="68"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="67"/>
-      <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L12" s="68"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="67"/>
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="68"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L13" s="68"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="67"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="68"/>
-      <c r="P14" s="68"/>
-      <c r="Q14" s="68"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L14" s="68"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="67"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="68"/>
-      <c r="P15" s="68"/>
-      <c r="Q15" s="68"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L15" s="68"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="67"/>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="68"/>
-      <c r="O16" s="68"/>
-      <c r="P16" s="68"/>
-      <c r="Q16" s="68"/>
+      <c r="L16" s="68"/>
     </row>
     <row r="17" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="105"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="71"/>
-      <c r="P17" s="71"/>
-      <c r="Q17" s="68"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="100"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="100"/>
+      <c r="J17" s="100"/>
+      <c r="K17" s="100"/>
+      <c r="L17" s="101"/>
+      <c r="M17" s="70"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="23"/>
-      <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="68"/>
-      <c r="P18" s="68"/>
-      <c r="Q18" s="68"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="72"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
       <c r="L19" s="23"/>
-      <c r="M19" s="68"/>
-      <c r="N19" s="68"/>
-      <c r="O19" s="68"/>
-      <c r="P19" s="68"/>
-      <c r="Q19" s="68"/>
     </row>
     <row r="20" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="107" t="s">
+      <c r="A20" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="108"/>
-      <c r="C20" s="108"/>
-      <c r="D20" s="108"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="108"/>
-      <c r="G20" s="108"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="108"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="108"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="68"/>
-      <c r="P20" s="68"/>
-      <c r="Q20" s="68"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="103"/>
+      <c r="I20" s="103"/>
+      <c r="J20" s="103"/>
+      <c r="K20" s="103"/>
+      <c r="L20" s="104"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="107"/>
-      <c r="B21" s="108"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="108"/>
-      <c r="F21" s="108"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="108"/>
-      <c r="I21" s="108"/>
-      <c r="J21" s="108"/>
-      <c r="K21" s="108"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="68"/>
-      <c r="O21" s="68"/>
-      <c r="P21" s="68"/>
-      <c r="Q21" s="68"/>
+      <c r="A21" s="102"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="103"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="103"/>
+      <c r="K21" s="103"/>
+      <c r="L21" s="104"/>
     </row>
     <row r="22" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
-      <c r="B22" s="110" t="s">
+      <c r="B22" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="110"/>
-      <c r="D22" s="110"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="111"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="68"/>
-      <c r="Q22" s="68"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="105"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="106"/>
     </row>
     <row r="23" spans="1:17" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="73"/>
+      <c r="K23" s="73"/>
       <c r="L23" s="25"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="75"/>
-      <c r="O23" s="75"/>
-      <c r="P23" s="75"/>
-      <c r="Q23" s="68"/>
+      <c r="M23" s="74"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="74"/>
+      <c r="P23" s="74"/>
     </row>
     <row r="24" spans="1:17" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="112" t="str">
+      <c r="A24" s="107" t="str">
         <f>'Design (2)'!A2:J2</f>
         <v>Re-excavation of Amtiol Khal from km 0.000 to km 3.300  = 3.300  km at  Gangni Upazilla of Meherpur District under Meherpur WD Division , BWDB, Meherpur.</v>
       </c>
-      <c r="B24" s="105"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="105"/>
-      <c r="J24" s="105"/>
-      <c r="K24" s="105"/>
-      <c r="L24" s="106"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="76"/>
-      <c r="O24" s="76"/>
-      <c r="P24" s="76"/>
-      <c r="Q24" s="76"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
+      <c r="D24" s="100"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="100"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="101"/>
+      <c r="M24" s="75"/>
+      <c r="N24" s="75"/>
+      <c r="O24" s="75"/>
+      <c r="P24" s="75"/>
+      <c r="Q24" s="75"/>
     </row>
     <row r="25" spans="1:17" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="113"/>
-      <c r="B25" s="105"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
-      <c r="I25" s="105"/>
-      <c r="J25" s="105"/>
-      <c r="K25" s="105"/>
-      <c r="L25" s="106"/>
-      <c r="M25" s="76"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="76"/>
-      <c r="P25" s="76"/>
-      <c r="Q25" s="76"/>
+      <c r="A25" s="108"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="101"/>
+      <c r="M25" s="75"/>
+      <c r="N25" s="75"/>
+      <c r="O25" s="75"/>
+      <c r="P25" s="75"/>
+      <c r="Q25" s="75"/>
     </row>
     <row r="26" spans="1:17" ht="55.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="113"/>
-      <c r="B26" s="105"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="105"/>
-      <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
-      <c r="I26" s="105"/>
-      <c r="J26" s="105"/>
-      <c r="K26" s="105"/>
-      <c r="L26" s="106"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="76"/>
-      <c r="O26" s="76"/>
-      <c r="P26" s="76"/>
-      <c r="Q26" s="76"/>
+      <c r="A26" s="108"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="101"/>
+      <c r="M26" s="75"/>
+      <c r="N26" s="75"/>
+      <c r="O26" s="75"/>
+      <c r="P26" s="75"/>
+      <c r="Q26" s="75"/>
     </row>
     <row r="27" spans="1:17" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-      <c r="K27" s="78"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="77"/>
+      <c r="J27" s="77"/>
+      <c r="K27" s="77"/>
       <c r="L27" s="27"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="79"/>
-      <c r="O27" s="79"/>
-      <c r="P27" s="79"/>
-      <c r="Q27" s="79"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="78"/>
+      <c r="O27" s="78"/>
+      <c r="P27" s="78"/>
+      <c r="Q27" s="78"/>
     </row>
     <row r="28" spans="1:17" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="80"/>
-      <c r="H28" s="80"/>
-      <c r="I28" s="80"/>
-      <c r="J28" s="80"/>
-      <c r="K28" s="80"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="79"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="79"/>
+      <c r="K28" s="79"/>
       <c r="L28" s="28"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="76"/>
+      <c r="M28" s="75"/>
+      <c r="N28" s="75"/>
+      <c r="O28" s="75"/>
+      <c r="P28" s="75"/>
+      <c r="Q28" s="75"/>
     </row>
     <row r="29" spans="1:17" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
-      <c r="B29" s="77"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="78"/>
-      <c r="J29" s="78"/>
-      <c r="K29" s="78"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="77"/>
+      <c r="K29" s="77"/>
       <c r="L29" s="27"/>
-      <c r="M29" s="79"/>
-      <c r="N29" s="79"/>
-      <c r="O29" s="79"/>
-      <c r="P29" s="79"/>
-      <c r="Q29" s="79"/>
+      <c r="M29" s="78"/>
+      <c r="N29" s="78"/>
+      <c r="O29" s="78"/>
+      <c r="P29" s="78"/>
+      <c r="Q29" s="78"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="77"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="76"/>
       <c r="L30" s="29"/>
-      <c r="M30" s="68"/>
-      <c r="N30" s="68"/>
-      <c r="O30" s="68"/>
-      <c r="P30" s="68"/>
-      <c r="Q30" s="68"/>
     </row>
     <row r="31" spans="1:17" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
       <c r="L31" s="27"/>
-      <c r="M31" s="79"/>
-      <c r="N31" s="79"/>
-      <c r="O31" s="79"/>
-      <c r="P31" s="79"/>
-      <c r="Q31" s="79"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="78"/>
+      <c r="O31" s="78"/>
+      <c r="P31" s="78"/>
+      <c r="Q31" s="78"/>
     </row>
     <row r="32" spans="1:17" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A32" s="114"/>
-      <c r="B32" s="115"/>
-      <c r="C32" s="115"/>
-      <c r="D32" s="115"/>
-      <c r="E32" s="115"/>
-      <c r="F32" s="115"/>
-      <c r="G32" s="115"/>
-      <c r="H32" s="115"/>
-      <c r="I32" s="115"/>
-      <c r="J32" s="115"/>
-      <c r="K32" s="115"/>
-      <c r="L32" s="116"/>
-      <c r="M32" s="76"/>
-      <c r="N32" s="76"/>
-      <c r="O32" s="76"/>
-      <c r="P32" s="76"/>
-      <c r="Q32" s="76"/>
+      <c r="A32" s="109"/>
+      <c r="B32" s="110"/>
+      <c r="C32" s="110"/>
+      <c r="D32" s="110"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="110"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="111"/>
+      <c r="M32" s="75"/>
+      <c r="N32" s="75"/>
+      <c r="O32" s="75"/>
+      <c r="P32" s="75"/>
+      <c r="Q32" s="75"/>
     </row>
     <row r="33" spans="1:28" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="78"/>
-      <c r="K33" s="78"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
       <c r="L33" s="27"/>
-      <c r="M33" s="79"/>
-      <c r="N33" s="79"/>
-      <c r="O33" s="79"/>
-      <c r="P33" s="79"/>
-      <c r="Q33" s="79"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="78"/>
+      <c r="O33" s="78"/>
+      <c r="P33" s="78"/>
+      <c r="Q33" s="78"/>
     </row>
     <row r="34" spans="1:28" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="100"/>
-      <c r="I34" s="100"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="82"/>
-      <c r="M34" s="76"/>
-      <c r="N34" s="76"/>
-      <c r="O34" s="76"/>
-      <c r="P34" s="76"/>
-      <c r="Q34" s="76"/>
+      <c r="B34" s="94"/>
+      <c r="C34" s="94"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="94"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="94"/>
+      <c r="H34" s="95"/>
+      <c r="I34" s="95"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="76"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="75"/>
+      <c r="N34" s="75"/>
+      <c r="O34" s="75"/>
+      <c r="P34" s="75"/>
+      <c r="Q34" s="75"/>
     </row>
     <row r="35" spans="1:28" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="67"/>
-      <c r="B35" s="83"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="83"/>
-      <c r="K35" s="83"/>
-      <c r="L35" s="84"/>
-      <c r="M35" s="79"/>
-      <c r="N35" s="79"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="79"/>
-      <c r="Q35" s="79"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="81"/>
+      <c r="M35" s="78"/>
+      <c r="N35" s="78"/>
+      <c r="O35" s="78"/>
+      <c r="P35" s="78"/>
+      <c r="Q35" s="78"/>
     </row>
     <row r="36" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="85"/>
-      <c r="B36" s="83"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
-      <c r="G36" s="101" t="s">
+      <c r="A36" s="82"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="H36" s="101"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="84"/>
-      <c r="M36" s="79"/>
-      <c r="N36" s="79"/>
-      <c r="O36" s="79"/>
-      <c r="P36" s="79"/>
-      <c r="Q36" s="79"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="81"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="78"/>
+      <c r="O36" s="78"/>
+      <c r="P36" s="78"/>
+      <c r="Q36" s="78"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="85"/>
-      <c r="B37" s="83"/>
-      <c r="C37" s="83"/>
-      <c r="D37" s="83"/>
-      <c r="E37" s="83"/>
-      <c r="F37" s="83"/>
-      <c r="G37" s="101"/>
-      <c r="H37" s="101"/>
-      <c r="I37" s="83"/>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="84"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="68"/>
-      <c r="O37" s="68"/>
-      <c r="P37" s="68"/>
-      <c r="Q37" s="68"/>
+      <c r="A37" s="82"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="96"/>
+      <c r="H37" s="96"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="80"/>
+      <c r="L37" s="81"/>
     </row>
     <row r="38" spans="1:28" ht="9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="26"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="83"/>
+      <c r="D38" s="83"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="83"/>
+      <c r="J38" s="83"/>
+      <c r="K38" s="83"/>
       <c r="L38" s="30"/>
-      <c r="M38" s="88"/>
-      <c r="N38" s="88"/>
-      <c r="O38" s="88"/>
-      <c r="P38" s="88"/>
-      <c r="Q38" s="68"/>
+      <c r="M38" s="85"/>
+      <c r="N38" s="85"/>
+      <c r="O38" s="85"/>
+      <c r="P38" s="85"/>
     </row>
     <row r="39" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="26"/>
-      <c r="B39" s="89"/>
-      <c r="C39" s="89"/>
-      <c r="D39" s="89"/>
-      <c r="E39" s="89"/>
-      <c r="F39" s="89"/>
-      <c r="G39" s="89"/>
-      <c r="H39" s="89"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="81"/>
-      <c r="L39" s="82"/>
-      <c r="M39" s="90"/>
-      <c r="N39" s="68"/>
-      <c r="O39" s="68"/>
-      <c r="P39" s="68"/>
-      <c r="Q39" s="68"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="86"/>
+      <c r="J39" s="86"/>
+      <c r="K39" s="76"/>
+      <c r="L39" s="29"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="26"/>
-      <c r="B40" s="77"/>
-      <c r="C40" s="77"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="77"/>
-      <c r="F40" s="77"/>
-      <c r="G40" s="77"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="77"/>
-      <c r="J40" s="77"/>
-      <c r="K40" s="77"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="76"/>
+      <c r="I40" s="76"/>
+      <c r="J40" s="76"/>
+      <c r="K40" s="76"/>
       <c r="L40" s="29"/>
-      <c r="M40" s="68"/>
-      <c r="N40" s="68"/>
-      <c r="O40" s="68"/>
-      <c r="P40" s="68"/>
-      <c r="Q40" s="68"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
-      <c r="B41" s="77"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="77"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="77"/>
-      <c r="K41" s="77"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
       <c r="L41" s="29"/>
-      <c r="M41" s="68"/>
-      <c r="N41" s="68"/>
-      <c r="O41" s="68"/>
-      <c r="P41" s="68"/>
-      <c r="Q41" s="68"/>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="77"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="77"/>
-      <c r="I42" s="77"/>
-      <c r="J42" s="77"/>
-      <c r="K42" s="77"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
       <c r="L42" s="29"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="68"/>
-      <c r="O42" s="68"/>
-      <c r="P42" s="68"/>
-      <c r="Q42" s="68"/>
     </row>
     <row r="43" spans="1:28" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A43" s="26"/>
-      <c r="B43" s="77"/>
-      <c r="C43" s="91" t="s">
+      <c r="B43" s="76"/>
+      <c r="C43" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="91"/>
-      <c r="H43" s="91"/>
-      <c r="I43" s="91"/>
-      <c r="J43" s="91"/>
-      <c r="K43" s="91"/>
-      <c r="L43" s="92"/>
-      <c r="M43" s="91"/>
-      <c r="N43" s="91"/>
-      <c r="O43" s="91"/>
-      <c r="P43" s="91"/>
-      <c r="Q43" s="91"/>
-      <c r="R43" s="91"/>
-      <c r="S43" s="91"/>
-      <c r="T43" s="91"/>
-      <c r="U43" s="91"/>
-      <c r="V43" s="91"/>
-      <c r="W43" s="91"/>
-      <c r="X43" s="91"/>
-      <c r="Y43" s="91"/>
-      <c r="Z43" s="91"/>
-      <c r="AA43" s="93"/>
-      <c r="AB43" s="93"/>
+      <c r="D43" s="87"/>
+      <c r="E43" s="87"/>
+      <c r="F43" s="87"/>
+      <c r="G43" s="87"/>
+      <c r="H43" s="87"/>
+      <c r="I43" s="87"/>
+      <c r="J43" s="87"/>
+      <c r="K43" s="87"/>
+      <c r="L43" s="88"/>
+      <c r="M43" s="87"/>
+      <c r="N43" s="87"/>
+      <c r="O43" s="87"/>
+      <c r="P43" s="87"/>
+      <c r="Q43" s="87"/>
+      <c r="R43" s="87"/>
+      <c r="S43" s="87"/>
+      <c r="T43" s="87"/>
+      <c r="U43" s="87"/>
+      <c r="V43" s="87"/>
+      <c r="W43" s="87"/>
+      <c r="X43" s="87"/>
+      <c r="Y43" s="87"/>
+      <c r="Z43" s="87"/>
+      <c r="AA43" s="89"/>
+      <c r="AB43" s="89"/>
     </row>
     <row r="44" spans="1:28" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A44" s="26"/>
-      <c r="B44" s="77"/>
-      <c r="C44" s="91" t="s">
+      <c r="B44" s="76"/>
+      <c r="C44" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="91"/>
-      <c r="E44" s="91"/>
-      <c r="F44" s="91"/>
-      <c r="G44" s="91"/>
-      <c r="H44" s="91"/>
-      <c r="I44" s="91"/>
-      <c r="J44" s="91"/>
-      <c r="K44" s="91"/>
-      <c r="L44" s="92"/>
-      <c r="M44" s="91"/>
-      <c r="N44" s="91"/>
-      <c r="O44" s="91"/>
-      <c r="P44" s="91"/>
-      <c r="Q44" s="91"/>
-      <c r="R44" s="91"/>
-      <c r="S44" s="91"/>
-      <c r="T44" s="91"/>
-      <c r="U44" s="91"/>
-      <c r="V44" s="91"/>
-      <c r="W44" s="91"/>
-      <c r="X44" s="91"/>
-      <c r="Y44" s="91"/>
-      <c r="Z44" s="91"/>
-      <c r="AA44" s="91"/>
-      <c r="AB44" s="91"/>
+      <c r="D44" s="87"/>
+      <c r="E44" s="87"/>
+      <c r="F44" s="87"/>
+      <c r="G44" s="87"/>
+      <c r="H44" s="87"/>
+      <c r="I44" s="87"/>
+      <c r="J44" s="87"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="88"/>
+      <c r="M44" s="87"/>
+      <c r="N44" s="87"/>
+      <c r="O44" s="87"/>
+      <c r="P44" s="87"/>
+      <c r="Q44" s="87"/>
+      <c r="R44" s="87"/>
+      <c r="S44" s="87"/>
+      <c r="T44" s="87"/>
+      <c r="U44" s="87"/>
+      <c r="V44" s="87"/>
+      <c r="W44" s="87"/>
+      <c r="X44" s="87"/>
+      <c r="Y44" s="87"/>
+      <c r="Z44" s="87"/>
+      <c r="AA44" s="87"/>
+      <c r="AB44" s="87"/>
     </row>
     <row r="45" spans="1:28" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A45" s="26"/>
-      <c r="B45" s="77"/>
-      <c r="C45" s="91" t="s">
+      <c r="B45" s="76"/>
+      <c r="C45" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="D45" s="91"/>
-      <c r="E45" s="91"/>
-      <c r="F45" s="91"/>
-      <c r="G45" s="91"/>
-      <c r="H45" s="91"/>
-      <c r="I45" s="91"/>
-      <c r="J45" s="91"/>
-      <c r="K45" s="91"/>
-      <c r="L45" s="92"/>
-      <c r="M45" s="91"/>
-      <c r="N45" s="91"/>
-      <c r="O45" s="91"/>
-      <c r="P45" s="91"/>
-      <c r="Q45" s="91"/>
-      <c r="R45" s="91"/>
-      <c r="S45" s="91"/>
-      <c r="T45" s="91"/>
-      <c r="U45" s="91"/>
-      <c r="V45" s="91"/>
-      <c r="W45" s="91"/>
-      <c r="X45" s="91"/>
-      <c r="Y45" s="91"/>
-      <c r="Z45" s="91"/>
-      <c r="AA45" s="94"/>
-      <c r="AB45" s="94"/>
+      <c r="D45" s="87"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="87"/>
+      <c r="H45" s="87"/>
+      <c r="I45" s="87"/>
+      <c r="J45" s="87"/>
+      <c r="K45" s="87"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="87"/>
+      <c r="N45" s="87"/>
+      <c r="O45" s="87"/>
+      <c r="P45" s="87"/>
+      <c r="Q45" s="87"/>
+      <c r="R45" s="87"/>
+      <c r="S45" s="87"/>
+      <c r="T45" s="87"/>
+      <c r="U45" s="87"/>
+      <c r="V45" s="87"/>
+      <c r="W45" s="87"/>
+      <c r="X45" s="87"/>
+      <c r="Y45" s="87"/>
+      <c r="Z45" s="87"/>
+      <c r="AA45" s="90"/>
+      <c r="AB45" s="90"/>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
-      <c r="B46" s="77"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
-      <c r="E46" s="77"/>
-      <c r="F46" s="77"/>
-      <c r="G46" s="77"/>
-      <c r="H46" s="77"/>
-      <c r="I46" s="77"/>
-      <c r="J46" s="77"/>
-      <c r="K46" s="77"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="76"/>
+      <c r="I46" s="76"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="76"/>
       <c r="L46" s="29"/>
-      <c r="M46" s="68"/>
-      <c r="N46" s="68"/>
-      <c r="O46" s="68"/>
-      <c r="P46" s="68"/>
-      <c r="Q46" s="68"/>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="26"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="77"/>
-      <c r="G47" s="77"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="77"/>
-      <c r="J47" s="77"/>
-      <c r="K47" s="77"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76"/>
       <c r="L47" s="29"/>
-      <c r="M47" s="68"/>
-      <c r="N47" s="68"/>
-      <c r="O47" s="68"/>
-      <c r="P47" s="68"/>
-      <c r="Q47" s="68"/>
     </row>
     <row r="48" spans="1:28" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="95"/>
-      <c r="B48" s="96"/>
-      <c r="C48" s="96"/>
-      <c r="D48" s="96"/>
-      <c r="E48" s="96"/>
-      <c r="F48" s="96"/>
-      <c r="G48" s="96"/>
-      <c r="H48" s="96"/>
-      <c r="I48" s="96"/>
-      <c r="J48" s="96"/>
-      <c r="K48" s="96"/>
-      <c r="L48" s="97"/>
-      <c r="M48" s="68"/>
-      <c r="N48" s="68"/>
-      <c r="O48" s="68"/>
-      <c r="P48" s="68"/>
-      <c r="Q48" s="68"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="68"/>
-      <c r="B49" s="68"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="68"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="68"/>
-      <c r="J49" s="68"/>
-      <c r="K49" s="68"/>
-      <c r="L49" s="68"/>
-      <c r="M49" s="68"/>
-      <c r="N49" s="68"/>
-      <c r="O49" s="68"/>
-      <c r="P49" s="68"/>
-      <c r="Q49" s="68"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A50" s="68"/>
-      <c r="B50" s="68"/>
-      <c r="C50" s="68"/>
-      <c r="D50" s="68"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="68"/>
-      <c r="H50" s="68"/>
-      <c r="I50" s="68"/>
-      <c r="J50" s="68"/>
-      <c r="K50" s="68"/>
-      <c r="L50" s="68"/>
-      <c r="M50" s="68"/>
-      <c r="N50" s="68"/>
-      <c r="O50" s="68"/>
-      <c r="P50" s="68"/>
-      <c r="Q50" s="68"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="68"/>
-      <c r="B51" s="68"/>
-      <c r="C51" s="68"/>
-      <c r="D51" s="68"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="68"/>
-      <c r="J51" s="68"/>
-      <c r="K51" s="68"/>
-      <c r="L51" s="68"/>
-      <c r="M51" s="68"/>
-      <c r="N51" s="68"/>
-      <c r="O51" s="68"/>
-      <c r="P51" s="68"/>
-      <c r="Q51" s="68"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="68"/>
-      <c r="B52" s="68"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="68"/>
-      <c r="E52" s="68"/>
-      <c r="F52" s="68"/>
-      <c r="G52" s="68"/>
-      <c r="H52" s="68"/>
-      <c r="I52" s="68"/>
-      <c r="J52" s="68"/>
-      <c r="K52" s="68"/>
-      <c r="L52" s="68"/>
-      <c r="M52" s="68"/>
-      <c r="N52" s="68"/>
-      <c r="O52" s="68"/>
-      <c r="P52" s="68"/>
-      <c r="Q52" s="68"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="68"/>
-      <c r="B53" s="68"/>
-      <c r="C53" s="68"/>
-      <c r="D53" s="68"/>
-      <c r="E53" s="68"/>
-      <c r="F53" s="68"/>
-      <c r="G53" s="68"/>
-      <c r="H53" s="68"/>
-      <c r="I53" s="68"/>
-      <c r="J53" s="68"/>
-      <c r="K53" s="68"/>
-      <c r="L53" s="68"/>
-      <c r="M53" s="68"/>
-      <c r="N53" s="68"/>
-      <c r="O53" s="68"/>
-      <c r="P53" s="68"/>
-      <c r="Q53" s="68"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="68"/>
-      <c r="B54" s="68"/>
-      <c r="C54" s="68"/>
-      <c r="D54" s="68"/>
-      <c r="E54" s="68"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="68"/>
-      <c r="J54" s="68"/>
-      <c r="K54" s="68"/>
-      <c r="L54" s="68"/>
-      <c r="M54" s="68"/>
-      <c r="N54" s="68"/>
-      <c r="O54" s="68"/>
-      <c r="P54" s="68"/>
-      <c r="Q54" s="68"/>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="68"/>
-      <c r="B55" s="68"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="68"/>
-      <c r="K55" s="68"/>
-      <c r="L55" s="68"/>
-      <c r="M55" s="68"/>
-      <c r="N55" s="68"/>
-      <c r="O55" s="68"/>
-      <c r="P55" s="68"/>
-      <c r="Q55" s="68"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A56" s="68"/>
-      <c r="B56" s="68"/>
-      <c r="C56" s="68"/>
-      <c r="D56" s="68"/>
-      <c r="E56" s="68"/>
-      <c r="F56" s="68"/>
-      <c r="G56" s="68"/>
-      <c r="H56" s="68"/>
-      <c r="I56" s="68"/>
-      <c r="J56" s="68"/>
-      <c r="K56" s="68"/>
-      <c r="L56" s="68"/>
-      <c r="M56" s="68"/>
-      <c r="N56" s="68"/>
-      <c r="O56" s="68"/>
-      <c r="P56" s="68"/>
-      <c r="Q56" s="68"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A57" s="68"/>
-      <c r="B57" s="68"/>
-      <c r="C57" s="68"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="68"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="68"/>
-      <c r="H57" s="68"/>
-      <c r="I57" s="68"/>
-      <c r="J57" s="68"/>
-      <c r="K57" s="68"/>
-      <c r="L57" s="68"/>
-      <c r="M57" s="68"/>
-      <c r="N57" s="68"/>
-      <c r="O57" s="68"/>
-      <c r="P57" s="68"/>
-      <c r="Q57" s="68"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" s="68"/>
-      <c r="B58" s="68"/>
-      <c r="C58" s="68"/>
-      <c r="D58" s="68"/>
-      <c r="E58" s="68"/>
-      <c r="F58" s="68"/>
-      <c r="G58" s="68"/>
-      <c r="H58" s="68"/>
-      <c r="I58" s="68"/>
-      <c r="J58" s="68"/>
-      <c r="K58" s="68"/>
-      <c r="L58" s="68"/>
-      <c r="M58" s="68"/>
-      <c r="N58" s="68"/>
-      <c r="O58" s="68"/>
-      <c r="P58" s="68"/>
-      <c r="Q58" s="68"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" s="68"/>
-      <c r="B59" s="68"/>
-      <c r="C59" s="68"/>
-      <c r="D59" s="68"/>
-      <c r="E59" s="68"/>
-      <c r="F59" s="68"/>
-      <c r="G59" s="68"/>
-      <c r="H59" s="68"/>
-      <c r="I59" s="68"/>
-      <c r="J59" s="68"/>
-      <c r="K59" s="68"/>
-      <c r="L59" s="68"/>
-      <c r="M59" s="68"/>
-      <c r="N59" s="68"/>
-      <c r="O59" s="68"/>
-      <c r="P59" s="68"/>
-      <c r="Q59" s="68"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" s="68"/>
-      <c r="B60" s="68"/>
-      <c r="C60" s="68"/>
-      <c r="D60" s="68"/>
-      <c r="E60" s="68"/>
-      <c r="F60" s="68"/>
-      <c r="G60" s="68"/>
-      <c r="H60" s="68"/>
-      <c r="I60" s="68"/>
-      <c r="J60" s="68"/>
-      <c r="K60" s="68"/>
-      <c r="L60" s="68"/>
-      <c r="M60" s="68"/>
-      <c r="N60" s="68"/>
-      <c r="O60" s="68"/>
-      <c r="P60" s="68"/>
-      <c r="Q60" s="68"/>
+      <c r="A48" s="91"/>
+      <c r="B48" s="92"/>
+      <c r="C48" s="92"/>
+      <c r="D48" s="92"/>
+      <c r="E48" s="92"/>
+      <c r="F48" s="92"/>
+      <c r="G48" s="92"/>
+      <c r="H48" s="92"/>
+      <c r="I48" s="92"/>
+      <c r="J48" s="92"/>
+      <c r="K48" s="92"/>
+      <c r="L48" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -17368,10 +16878,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M147"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="104" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A127" zoomScaleNormal="104" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="M104" sqref="M104"/>
     </sheetView>
   </sheetViews>
@@ -17393,25 +16903,25 @@
     <col min="20" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="121" t="s">
+    <row r="1" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-    </row>
-    <row r="2" spans="1:13" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="118" t="s">
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+    </row>
+    <row r="2" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="118"/>
+      <c r="B2" s="113"/>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
         <v>21</v>
@@ -17423,11 +16933,11 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="120"/>
+      <c r="B3" s="115"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -17437,7 +16947,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="43" t="s">
         <v>4</v>
       </c>
@@ -17453,7 +16963,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="45">
         <v>0</v>
       </c>
@@ -17469,7 +16979,7 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="45">
         <v>5</v>
       </c>
@@ -17485,7 +16995,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="45">
         <v>10</v>
       </c>
@@ -17501,7 +17011,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="45">
         <v>15</v>
       </c>
@@ -17517,7 +17027,7 @@
       <c r="I8" s="4"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="45">
         <v>20</v>
       </c>
@@ -17534,7 +17044,7 @@
       <c r="J9" s="4"/>
       <c r="M9" s="20"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="45">
         <v>25</v>
       </c>
@@ -17550,7 +17060,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="45">
         <v>30</v>
       </c>
@@ -17566,7 +17076,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="45">
         <v>35</v>
       </c>
@@ -17582,7 +17092,7 @@
       <c r="I12" s="7"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="45">
         <v>40</v>
       </c>
@@ -17598,7 +17108,7 @@
       <c r="I13" s="13"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="45">
         <v>41</v>
       </c>
@@ -17614,7 +17124,7 @@
       <c r="I14" s="4"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="45">
         <v>42</v>
       </c>
@@ -17630,7 +17140,7 @@
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="45">
         <v>43</v>
       </c>
@@ -17646,7 +17156,7 @@
       <c r="I16" s="4"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="45">
         <v>44</v>
       </c>
@@ -17662,7 +17172,7 @@
       <c r="I17" s="4"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="45">
         <v>45.5</v>
       </c>
@@ -17677,7 +17187,7 @@
       <c r="I18" s="17"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="45">
         <v>46</v>
       </c>
@@ -17690,7 +17200,7 @@
       <c r="I19" s="17"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="45">
         <v>47</v>
       </c>
@@ -17706,7 +17216,7 @@
       <c r="I20" s="17"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="45">
         <v>48</v>
       </c>
@@ -17721,7 +17231,7 @@
       <c r="I21" s="17"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="45">
         <v>49</v>
       </c>
@@ -17737,7 +17247,7 @@
       <c r="I22" s="17"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="45">
         <v>50</v>
       </c>
@@ -17753,7 +17263,7 @@
       <c r="I23" s="17"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="45">
         <v>51</v>
       </c>
@@ -17769,7 +17279,7 @@
       <c r="I24" s="17"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="45">
         <v>52</v>
       </c>
@@ -17785,7 +17295,7 @@
       <c r="I25" s="17"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="45">
         <v>53</v>
       </c>
@@ -17801,7 +17311,7 @@
       <c r="I26" s="17"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="45">
         <v>54</v>
       </c>
@@ -17817,7 +17327,7 @@
       <c r="I27" s="17"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="45">
         <v>55</v>
       </c>
@@ -17833,7 +17343,7 @@
       <c r="I28" s="17"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="45">
         <v>56</v>
       </c>
@@ -17849,7 +17359,7 @@
       <c r="I29" s="17"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="45">
         <v>57</v>
       </c>
@@ -17865,7 +17375,7 @@
       <c r="I30" s="17"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="45">
         <v>58</v>
       </c>
@@ -17881,7 +17391,7 @@
       <c r="I31" s="17"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="45">
         <v>59</v>
       </c>
@@ -17897,7 +17407,7 @@
       <c r="I32" s="17"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="45">
         <v>60</v>
       </c>
@@ -17913,7 +17423,7 @@
       <c r="I33" s="17"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="45">
         <v>61</v>
       </c>
@@ -17929,7 +17439,7 @@
       <c r="I34" s="17"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="45">
         <v>62</v>
       </c>
@@ -17945,7 +17455,7 @@
       <c r="I35" s="17"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="45">
         <v>63</v>
       </c>
@@ -17961,7 +17471,7 @@
       <c r="I36" s="17"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="45">
         <v>64</v>
       </c>
@@ -17977,7 +17487,7 @@
       <c r="I37" s="17"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="45">
         <v>65</v>
       </c>
@@ -17993,7 +17503,7 @@
       <c r="I38" s="17"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="45">
         <v>66</v>
       </c>
@@ -18009,7 +17519,7 @@
       <c r="I39" s="17"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="45">
         <v>67</v>
       </c>
@@ -18025,7 +17535,7 @@
       <c r="I40" s="17"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="45">
         <v>68</v>
       </c>
@@ -18041,7 +17551,7 @@
       <c r="I41" s="17"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="45">
         <v>69</v>
       </c>
@@ -18057,7 +17567,7 @@
       <c r="I42" s="17"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="45">
         <v>70</v>
       </c>
@@ -18073,7 +17583,7 @@
       <c r="I43" s="17"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="45">
         <v>71</v>
       </c>
@@ -18346,10 +17856,10 @@
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="118" t="s">
+      <c r="A76" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="118"/>
+      <c r="B76" s="113"/>
       <c r="C76" s="3"/>
       <c r="D76" s="2" t="s">
         <v>22</v>
@@ -18362,10 +17872,10 @@
       <c r="J76" s="3"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A77" s="117" t="s">
+      <c r="A77" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="B77" s="117"/>
+      <c r="B77" s="112"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -19512,11 +19022,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O301"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A43" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="L59" sqref="L59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -19535,31 +19045,31 @@
   <sheetData>
     <row r="1" spans="1:15" ht="7.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="124" t="s">
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="125"/>
+      <c r="B3" s="119"/>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="126" t="s">
+      <c r="I3" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="127"/>
+      <c r="J3" s="121"/>
     </row>
     <row r="4" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
@@ -19897,10 +19407,10 @@
       <c r="O30" s="36"/>
     </row>
     <row r="31" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="124" t="s">
+      <c r="A31" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="125"/>
+      <c r="B31" s="119"/>
       <c r="E31" s="34"/>
       <c r="G31" s="35"/>
       <c r="N31" s="36"/>
@@ -19916,10 +19426,10 @@
       <c r="E32" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I32" s="126" t="s">
+      <c r="I32" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J32" s="127"/>
+      <c r="J32" s="121"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
     </row>
@@ -20123,10 +19633,10 @@
       <c r="B51" s="56"/>
     </row>
     <row r="52" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="124" t="s">
+      <c r="A52" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="125"/>
+      <c r="B52" s="119"/>
     </row>
     <row r="53" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="53" t="s">
@@ -20135,15 +19645,15 @@
       <c r="B53" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="118" t="s">
+      <c r="C53" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="118"/>
-      <c r="E53" s="118"/>
-      <c r="I53" s="126" t="s">
+      <c r="D53" s="113"/>
+      <c r="E53" s="113"/>
+      <c r="I53" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J53" s="127"/>
+      <c r="J53" s="121"/>
     </row>
     <row r="54" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="53">
@@ -20326,14 +19836,14 @@
       <c r="J67" s="58"/>
     </row>
     <row r="68" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="124" t="s">
+      <c r="A68" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B68" s="125"/>
-      <c r="I68" s="126" t="s">
+      <c r="B68" s="119"/>
+      <c r="I68" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J68" s="127"/>
+      <c r="J68" s="121"/>
     </row>
     <row r="69" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="53" t="s">
@@ -20342,11 +19852,11 @@
       <c r="B69" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="118" t="s">
+      <c r="C69" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="118"/>
-      <c r="E69" s="118"/>
+      <c r="D69" s="113"/>
+      <c r="E69" s="113"/>
       <c r="I69" s="53" t="s">
         <v>1</v>
       </c>
@@ -20565,10 +20075,10 @@
       <c r="B88" s="56"/>
     </row>
     <row r="89" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="124" t="s">
+      <c r="A89" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="125"/>
+      <c r="B89" s="119"/>
     </row>
     <row r="90" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="53" t="s">
@@ -20577,15 +20087,15 @@
       <c r="B90" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C90" s="118" t="s">
+      <c r="C90" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="D90" s="118"/>
-      <c r="E90" s="118"/>
-      <c r="I90" s="126" t="s">
+      <c r="D90" s="113"/>
+      <c r="E90" s="113"/>
+      <c r="I90" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J90" s="127"/>
+      <c r="J90" s="121"/>
     </row>
     <row r="91" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="53">
@@ -20792,10 +20302,10 @@
       <c r="B108" s="56"/>
     </row>
     <row r="109" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="124" t="s">
+      <c r="A109" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B109" s="125"/>
+      <c r="B109" s="119"/>
     </row>
     <row r="110" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="53" t="s">
@@ -20804,15 +20314,15 @@
       <c r="B110" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C110" s="118" t="s">
+      <c r="C110" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="D110" s="118"/>
-      <c r="E110" s="118"/>
-      <c r="I110" s="126" t="s">
+      <c r="D110" s="113"/>
+      <c r="E110" s="113"/>
+      <c r="I110" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J110" s="127"/>
+      <c r="J110" s="121"/>
     </row>
     <row r="111" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="53">
@@ -21089,14 +20599,14 @@
       <c r="B132" s="56"/>
     </row>
     <row r="133" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="124" t="s">
+      <c r="A133" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B133" s="125"/>
-      <c r="I133" s="126" t="s">
+      <c r="B133" s="119"/>
+      <c r="I133" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J133" s="127"/>
+      <c r="J133" s="121"/>
     </row>
     <row r="134" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="53" t="s">
@@ -21105,11 +20615,11 @@
       <c r="B134" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C134" s="118" t="s">
+      <c r="C134" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="D134" s="118"/>
-      <c r="E134" s="118"/>
+      <c r="D134" s="113"/>
+      <c r="E134" s="113"/>
       <c r="I134" s="53" t="s">
         <v>1</v>
       </c>
@@ -21350,8 +20860,8 @@
       <c r="J152" s="56"/>
     </row>
     <row r="153" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="98"/>
-      <c r="B153" s="98"/>
+      <c r="A153" s="56"/>
+      <c r="B153" s="56"/>
       <c r="I153" s="56"/>
       <c r="J153" s="56"/>
     </row>
@@ -21362,19 +20872,19 @@
       <c r="J154" s="56"/>
     </row>
     <row r="155" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="124" t="s">
+      <c r="A155" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B155" s="125"/>
-      <c r="C155" s="118" t="s">
+      <c r="B155" s="119"/>
+      <c r="C155" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="D155" s="118"/>
-      <c r="E155" s="118"/>
-      <c r="I155" s="126" t="s">
+      <c r="D155" s="113"/>
+      <c r="E155" s="113"/>
+      <c r="I155" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J155" s="127"/>
+      <c r="J155" s="121"/>
     </row>
     <row r="156" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="53" t="s">
@@ -21611,8 +21121,8 @@
       <c r="J173" s="56"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A174" s="98"/>
-      <c r="B174" s="98"/>
+      <c r="A174" s="56"/>
+      <c r="B174" s="56"/>
       <c r="I174" s="56"/>
       <c r="J174" s="56"/>
     </row>
@@ -21621,19 +21131,19 @@
       <c r="J175" s="56"/>
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A176" s="124" t="s">
+      <c r="A176" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B176" s="125"/>
-      <c r="C176" s="118" t="s">
+      <c r="B176" s="119"/>
+      <c r="C176" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="D176" s="118"/>
-      <c r="E176" s="118"/>
-      <c r="I176" s="126" t="s">
+      <c r="D176" s="113"/>
+      <c r="E176" s="113"/>
+      <c r="I176" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J176" s="127"/>
+      <c r="J176" s="121"/>
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="53" t="s">
@@ -21884,19 +21394,19 @@
       </c>
     </row>
     <row r="197" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A197" s="124" t="s">
+      <c r="A197" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B197" s="125"/>
-      <c r="C197" s="118" t="s">
+      <c r="B197" s="119"/>
+      <c r="C197" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="D197" s="118"/>
-      <c r="E197" s="118"/>
-      <c r="I197" s="126" t="s">
+      <c r="D197" s="113"/>
+      <c r="E197" s="113"/>
+      <c r="I197" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J197" s="127"/>
+      <c r="J197" s="121"/>
     </row>
     <row r="198" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="53" t="s">
@@ -22154,19 +21664,19 @@
     </row>
     <row r="219" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="220" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="124" t="s">
+      <c r="A220" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B220" s="125"/>
-      <c r="C220" s="118" t="s">
+      <c r="B220" s="119"/>
+      <c r="C220" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="D220" s="118"/>
-      <c r="E220" s="118"/>
-      <c r="I220" s="126" t="s">
+      <c r="D220" s="113"/>
+      <c r="E220" s="113"/>
+      <c r="I220" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J220" s="127"/>
+      <c r="J220" s="121"/>
     </row>
     <row r="221" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="53" t="s">
@@ -22349,19 +21859,19 @@
       <c r="J234" s="56"/>
     </row>
     <row r="235" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="124" t="s">
+      <c r="A235" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B235" s="125"/>
-      <c r="C235" s="118" t="s">
+      <c r="B235" s="119"/>
+      <c r="C235" s="113" t="s">
         <v>32</v>
       </c>
-      <c r="D235" s="118"/>
-      <c r="E235" s="118"/>
-      <c r="I235" s="126" t="s">
+      <c r="D235" s="113"/>
+      <c r="E235" s="113"/>
+      <c r="I235" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J235" s="127"/>
+      <c r="J235" s="121"/>
     </row>
     <row r="236" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="53" t="s">
@@ -22602,19 +22112,19 @@
       <c r="J254" s="56"/>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A256" s="124" t="s">
+      <c r="A256" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B256" s="125"/>
-      <c r="C256" s="118" t="s">
+      <c r="B256" s="119"/>
+      <c r="C256" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="D256" s="118"/>
-      <c r="E256" s="118"/>
-      <c r="I256" s="126" t="s">
+      <c r="D256" s="113"/>
+      <c r="E256" s="113"/>
+      <c r="I256" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J256" s="127"/>
+      <c r="J256" s="121"/>
     </row>
     <row r="257" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A257" s="53" t="s">
@@ -22871,19 +22381,19 @@
       </c>
     </row>
     <row r="278" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A278" s="124" t="s">
+      <c r="A278" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B278" s="125"/>
-      <c r="C278" s="118" t="s">
+      <c r="B278" s="119"/>
+      <c r="C278" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="D278" s="118"/>
-      <c r="E278" s="118"/>
-      <c r="I278" s="126" t="s">
+      <c r="D278" s="113"/>
+      <c r="E278" s="113"/>
+      <c r="I278" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="J278" s="127"/>
+      <c r="J278" s="121"/>
     </row>
     <row r="279" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A279" s="53" t="s">
@@ -23075,39 +22585,8 @@
       <c r="O301" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="A256:B256"/>
-    <mergeCell ref="C256:E256"/>
-    <mergeCell ref="I256:J256"/>
-    <mergeCell ref="A278:B278"/>
-    <mergeCell ref="C278:E278"/>
-    <mergeCell ref="I278:J278"/>
-    <mergeCell ref="A220:B220"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="I220:J220"/>
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="C235:E235"/>
-    <mergeCell ref="I235:J235"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="C176:E176"/>
-    <mergeCell ref="I176:J176"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="I197:J197"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="I133:J133"/>
-    <mergeCell ref="C134:E134"/>
-    <mergeCell ref="A155:B155"/>
-    <mergeCell ref="C155:E155"/>
-    <mergeCell ref="I155:J155"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="I90:J90"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="I110:J110"/>
+  <mergeCells count="40">
     <mergeCell ref="C69:E69"/>
-    <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="A31:B31"/>
@@ -23117,6 +22596,36 @@
     <mergeCell ref="I53:J53"/>
     <mergeCell ref="A68:B68"/>
     <mergeCell ref="I68:J68"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="I90:J90"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="C110:E110"/>
+    <mergeCell ref="I110:J110"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="I133:J133"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="A155:B155"/>
+    <mergeCell ref="C155:E155"/>
+    <mergeCell ref="I155:J155"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="I176:J176"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="I197:J197"/>
+    <mergeCell ref="A220:B220"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="I220:J220"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="C235:E235"/>
+    <mergeCell ref="I235:J235"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="C256:E256"/>
+    <mergeCell ref="I256:J256"/>
+    <mergeCell ref="A278:B278"/>
+    <mergeCell ref="C278:E278"/>
+    <mergeCell ref="I278:J278"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>
@@ -23129,10 +22638,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
@@ -23149,34 +22658,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
-      <c r="P1" s="128"/>
-      <c r="Q1" s="128"/>
-      <c r="R1" s="128"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="128"/>
-      <c r="U1" s="128"/>
-      <c r="V1" s="128"/>
-      <c r="W1" s="128"/>
-      <c r="X1" s="128"/>
-      <c r="Y1" s="128"/>
-      <c r="Z1" s="128"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
+      <c r="P1" s="122"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="122"/>
+      <c r="T1" s="122"/>
+      <c r="U1" s="122"/>
+      <c r="V1" s="122"/>
+      <c r="W1" s="122"/>
+      <c r="X1" s="122"/>
+      <c r="Y1" s="122"/>
+      <c r="Z1" s="122"/>
       <c r="AA1" s="40"/>
       <c r="AB1" s="40"/>
       <c r="AC1" s="40"/>
@@ -23186,35 +22695,35 @@
       <c r="AG1" s="40"/>
       <c r="AH1" s="40"/>
     </row>
-    <row r="2" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="129" t="s">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="123" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="129"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="129"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="129"/>
-      <c r="S2" s="129"/>
-      <c r="T2" s="129"/>
-      <c r="U2" s="129"/>
-      <c r="V2" s="129"/>
-      <c r="W2" s="129"/>
-      <c r="X2" s="129"/>
-      <c r="Y2" s="129"/>
-      <c r="Z2" s="129"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="123"/>
+      <c r="D2" s="123"/>
+      <c r="E2" s="123"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="123"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="123"/>
+      <c r="Q2" s="123"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="123"/>
+      <c r="T2" s="123"/>
+      <c r="U2" s="123"/>
+      <c r="V2" s="123"/>
+      <c r="W2" s="123"/>
+      <c r="X2" s="123"/>
+      <c r="Y2" s="123"/>
+      <c r="Z2" s="123"/>
       <c r="AA2" s="42"/>
       <c r="AB2" s="41"/>
       <c r="AC2" s="41"/>

</xml_diff>